<commit_message>
Corrected Jaye Robinson data
</commit_message>
<xml_diff>
--- a/utils/similarity_chw.xlsx
+++ b/utils/similarity_chw.xlsx
@@ -19097,7 +19097,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD30"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19218,7 +19218,7 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Jaye Robinson</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
@@ -19244,11 +19244,6 @@
       <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Gary Crawford</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Jaye Robinson</t>
         </is>
       </c>
     </row>
@@ -19338,7 +19333,6 @@
       </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -19413,7 +19407,7 @@
         <v>0.6170212765957447</v>
       </c>
       <c r="X3" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="Y3" t="n">
         <v>0.5490196078431373</v>
@@ -19429,9 +19423,6 @@
       </c>
       <c r="AC3" t="n">
         <v>0.5</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="4">
@@ -19507,7 +19498,7 @@
         <v>0.6956521739130435</v>
       </c>
       <c r="X4" t="n">
-        <v>0.6521739130434783</v>
+        <v>0.5862068965517242</v>
       </c>
       <c r="Y4" t="n">
         <v>0.64</v>
@@ -19523,9 +19514,6 @@
       </c>
       <c r="AC4" t="n">
         <v>0.875</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="5">
@@ -19601,7 +19589,7 @@
         <v>0.6666666666666667</v>
       </c>
       <c r="X5" t="n">
-        <v>0.65</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="Y5" t="n">
         <v>0.6170212765957447</v>
@@ -19617,9 +19605,6 @@
       </c>
       <c r="AC5" t="n">
         <v>0.625</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0.6666666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -19695,7 +19680,7 @@
         <v>0.736842105263158</v>
       </c>
       <c r="X6" t="n">
-        <v>0.6875</v>
+        <v>0.6818181818181819</v>
       </c>
       <c r="Y6" t="n">
         <v>0.6829268292682926</v>
@@ -19711,9 +19696,6 @@
       </c>
       <c r="AC6" t="n">
         <v>0.875</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0.6666666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -19789,7 +19771,7 @@
         <v>0.5800000000000001</v>
       </c>
       <c r="X7" t="n">
-        <v>0.5652173913043479</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="Y7" t="n">
         <v>0.5094339622641509</v>
@@ -19805,9 +19787,6 @@
       </c>
       <c r="AC7" t="n">
         <v>0.25</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="8">
@@ -19883,7 +19862,7 @@
         <v>0.5918367346938775</v>
       </c>
       <c r="X8" t="n">
-        <v>0.5652173913043479</v>
+        <v>0.5172413793103448</v>
       </c>
       <c r="Y8" t="n">
         <v>0.5576923076923077</v>
@@ -19899,9 +19878,6 @@
       </c>
       <c r="AC8" t="n">
         <v>0.375</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="9">
@@ -19977,7 +19953,7 @@
         <v>0.5800000000000001</v>
       </c>
       <c r="X9" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.5862068965517242</v>
       </c>
       <c r="Y9" t="n">
         <v>0.5</v>
@@ -19993,9 +19969,6 @@
       </c>
       <c r="AC9" t="n">
         <v>0.25</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="10">
@@ -20071,7 +20044,7 @@
         <v>0.6326530612244898</v>
       </c>
       <c r="X10" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="Y10" t="n">
         <v>0.5576923076923077</v>
@@ -20087,9 +20060,6 @@
       </c>
       <c r="AC10" t="n">
         <v>0.4285714285714286</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>0.4</v>
       </c>
     </row>
     <row r="11">
@@ -20165,7 +20135,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="X11" t="n">
-        <v>0.5217391304347826</v>
+        <v>0.5172413793103448</v>
       </c>
       <c r="Y11" t="n">
         <v>0.4905660377358491</v>
@@ -20181,9 +20151,6 @@
       </c>
       <c r="AC11" t="n">
         <v>0.25</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="12">
@@ -20259,7 +20226,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="X12" t="n">
-        <v>0.5652173913043479</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="Y12" t="n">
         <v>0.4905660377358491</v>
@@ -20275,9 +20242,6 @@
       </c>
       <c r="AC12" t="n">
         <v>0.25</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="13">
@@ -20353,7 +20317,7 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="X13" t="n">
-        <v>0.5652173913043479</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="Y13" t="n">
         <v>0.4905660377358491</v>
@@ -20369,9 +20333,6 @@
       </c>
       <c r="AC13" t="n">
         <v>0.25</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="14">
@@ -20447,7 +20408,7 @@
         <v>0.7391304347826086</v>
       </c>
       <c r="X14" t="n">
-        <v>0.6818181818181819</v>
+        <v>0.6071428571428572</v>
       </c>
       <c r="Y14" t="n">
         <v>0.7142857142857143</v>
@@ -20463,9 +20424,6 @@
       </c>
       <c r="AC14" t="n">
         <v>0.875</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="15">
@@ -20558,9 +20516,6 @@
       <c r="AC15" t="n">
         <v>0.25</v>
       </c>
-      <c r="AD15" t="n">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -20635,7 +20590,7 @@
         <v>0.5957446808510638</v>
       </c>
       <c r="X16" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="Y16" t="n">
         <v>0.5918367346938775</v>
@@ -20651,9 +20606,6 @@
       </c>
       <c r="AC16" t="n">
         <v>0.625</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="17">
@@ -20742,7 +20694,6 @@
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -20817,7 +20768,7 @@
         <v>0.6122448979591837</v>
       </c>
       <c r="X18" t="n">
-        <v>0.6521739130434783</v>
+        <v>0.5862068965517242</v>
       </c>
       <c r="Y18" t="n">
         <v>0.5294117647058824</v>
@@ -20833,9 +20784,6 @@
       </c>
       <c r="AC18" t="n">
         <v>0.375</v>
-      </c>
-      <c r="AD18" t="n">
-        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="19">
@@ -20911,7 +20859,7 @@
         <v>0.78</v>
       </c>
       <c r="X19" t="n">
-        <v>0.6521739130434783</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="Y19" t="n">
         <v>0.7169811320754718</v>
@@ -20927,9 +20875,6 @@
       </c>
       <c r="AC19" t="n">
         <v>1</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="20">
@@ -21005,7 +20950,7 @@
         <v>0.7173913043478262</v>
       </c>
       <c r="X20" t="n">
-        <v>0.6190476190476191</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="Y20" t="n">
         <v>0.7551020408163265</v>
@@ -21021,9 +20966,6 @@
       </c>
       <c r="AC20" t="n">
         <v>0.875</v>
-      </c>
-      <c r="AD20" t="n">
-        <v>0.6666666666666667</v>
       </c>
     </row>
     <row r="21">
@@ -21099,7 +21041,7 @@
         <v>0.6170212765957447</v>
       </c>
       <c r="X21" t="n">
-        <v>0.65</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="Y21" t="n">
         <v>0.5319148936170213</v>
@@ -21115,9 +21057,6 @@
       </c>
       <c r="AC21" t="n">
         <v>0.2857142857142857</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="22">
@@ -21193,7 +21132,7 @@
         <v>0.7804878048780488</v>
       </c>
       <c r="X22" t="n">
-        <v>0.7333333333333334</v>
+        <v>0.7</v>
       </c>
       <c r="Y22" t="n">
         <v>0.6590909090909092</v>
@@ -21209,9 +21148,6 @@
       </c>
       <c r="AC22" t="n">
         <v>0.7142857142857143</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>0.6</v>
       </c>
     </row>
     <row r="23">
@@ -21287,7 +21223,7 @@
         <v>1</v>
       </c>
       <c r="X23" t="n">
-        <v>0.8571428571428572</v>
+        <v>0.8148148148148149</v>
       </c>
       <c r="Y23" t="n">
         <v>0.6875</v>
@@ -21303,98 +21239,98 @@
       </c>
       <c r="AC23" t="n">
         <v>0.875</v>
-      </c>
-      <c r="AD23" t="n">
-        <v>0.6666666666666667</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Jaye Robinson</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>0.6086956521739131</v>
       </c>
       <c r="C24" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6521739130434783</v>
+        <v>0.5862068965517242</v>
       </c>
       <c r="E24" t="n">
-        <v>0.65</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="F24" t="n">
-        <v>0.6875</v>
+        <v>0.6818181818181819</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5652173913043479</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="H24" t="n">
-        <v>0.5652173913043479</v>
+        <v>0.5172413793103448</v>
       </c>
       <c r="I24" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.5862068965517242</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="K24" t="n">
-        <v>0.5217391304347826</v>
+        <v>0.5172413793103448</v>
       </c>
       <c r="L24" t="n">
-        <v>0.5652173913043479</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="M24" t="n">
-        <v>0.5652173913043479</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="N24" t="n">
-        <v>0.6818181818181819</v>
+        <v>0.6071428571428572</v>
       </c>
       <c r="O24" t="n">
         <v>0.5</v>
       </c>
       <c r="P24" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="Q24" t="n">
         <v>0.7</v>
       </c>
       <c r="R24" t="n">
-        <v>0.6521739130434783</v>
+        <v>0.5862068965517242</v>
       </c>
       <c r="S24" t="n">
-        <v>0.6521739130434783</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="T24" t="n">
-        <v>0.6190476190476191</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="U24" t="n">
-        <v>0.65</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="V24" t="n">
-        <v>0.7333333333333334</v>
+        <v>0.7</v>
       </c>
       <c r="W24" t="n">
-        <v>0.8571428571428572</v>
+        <v>0.8148148148148149</v>
       </c>
       <c r="X24" t="n">
         <v>1</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.7391304347826086</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.6153846153846154</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.5217391304347826</v>
-      </c>
-      <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="inlineStr"/>
-      <c r="AD24" t="inlineStr"/>
+        <v>0.5172413793103448</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -21469,7 +21405,7 @@
         <v>0.6875</v>
       </c>
       <c r="X25" t="n">
-        <v>0.7391304347826086</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="Y25" t="n">
         <v>1</v>
@@ -21485,9 +21421,6 @@
       </c>
       <c r="AC25" t="n">
         <v>0.875</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="26">
@@ -21563,7 +21496,7 @@
         <v>0.7692307692307692</v>
       </c>
       <c r="X26" t="n">
-        <v>0.6153846153846154</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="Y26" t="n">
         <v>0.7</v>
@@ -21579,9 +21512,6 @@
       </c>
       <c r="AC26" t="n">
         <v>1</v>
-      </c>
-      <c r="AD26" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="27">
@@ -21657,7 +21587,7 @@
         <v>0.4399999999999999</v>
       </c>
       <c r="X27" t="n">
-        <v>0.5217391304347826</v>
+        <v>0.5172413793103448</v>
       </c>
       <c r="Y27" t="n">
         <v>0.5471698113207547</v>
@@ -21673,9 +21603,6 @@
       </c>
       <c r="AC27" t="n">
         <v>0.375</v>
-      </c>
-      <c r="AD27" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="28">
@@ -21746,7 +21673,9 @@
       <c r="W28" t="n">
         <v>0.875</v>
       </c>
-      <c r="X28" t="inlineStr"/>
+      <c r="X28" t="n">
+        <v>0.5</v>
+      </c>
       <c r="Y28" t="n">
         <v>0.875</v>
       </c>
@@ -21761,9 +21690,6 @@
       </c>
       <c r="AC28" t="n">
         <v>1</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="29">
@@ -21834,7 +21760,9 @@
       <c r="W29" t="n">
         <v>0.875</v>
       </c>
-      <c r="X29" t="inlineStr"/>
+      <c r="X29" t="n">
+        <v>0.5</v>
+      </c>
       <c r="Y29" t="n">
         <v>0.875</v>
       </c>
@@ -21848,97 +21776,6 @@
         <v>1</v>
       </c>
       <c r="AC29" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD29" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Jaye Robinson</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="n">
-        <v>0.3333333333333334</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.3333333333333334</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.6666666666666667</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.6666666666666667</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0.3333333333333334</v>
-      </c>
-      <c r="I30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J30" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N30" t="n">
-        <v>0.3333333333333334</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="n">
-        <v>0.3333333333333334</v>
-      </c>
-      <c r="S30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="T30" t="n">
-        <v>0.6666666666666667</v>
-      </c>
-      <c r="U30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="V30" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="W30" t="n">
-        <v>0.6666666666666667</v>
-      </c>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="n">
-        <v>0.3333333333333334</v>
-      </c>
-      <c r="Z30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AA30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AB30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AC30" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AD30" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>